<commit_message>
Plotted pH 9 PYR data
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaPYR_pH7/RaPYR_pH7_NoScript.xlsx
+++ b/Sorption Experiments/RaPYR_pH7/RaPYR_pH7_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -838,11 +838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91385392"/>
-        <c:axId val="91384608"/>
+        <c:axId val="496290160"/>
+        <c:axId val="496285456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91385392"/>
+        <c:axId val="496290160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,12 +870,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91384608"/>
+        <c:crossAx val="496285456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91384608"/>
+        <c:axId val="496285456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,7 +903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91385392"/>
+        <c:crossAx val="496290160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5961,7 +5961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D19"/>
     </sheetView>
   </sheetViews>
@@ -7929,7 +7929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>